<commit_message>
corrected for missing LC+N+S character rule
</commit_message>
<xml_diff>
--- a/assets/charset dupe checker.xlsx
+++ b/assets/charset dupe checker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\bootcamp\upenn-bootcamp\js-password-generator\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ECAEC7B-3A39-47BF-9684-9E9E34F49900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30921F40-DBF7-45B2-8A28-1B9530E83771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12315" yWindow="2610" windowWidth="15990" windowHeight="10860" xr2:uid="{FFE0A6B3-15AF-4E34-BB0E-08843EEF7F3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFE0A6B3-15AF-4E34-BB0E-08843EEF7F3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,17 +98,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -442,7 +432,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,8 +689,8 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>